<commit_message>
do a diff before updating comments. closes #10
</commit_message>
<xml_diff>
--- a/fexcel/testdata/test.xlsx
+++ b/fexcel/testdata/test.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jay\dev\go\src\github.com\onerobotics\fexcel\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/dev/go/src/github.com/onerobotics/fexcel/fexcel/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46CE69B-B93E-4CCE-AB01-2998203447ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="264" yWindow="1128" windowWidth="12612" windowHeight="11292" xr2:uid="{A83EBFEA-4CE7-42E2-83DE-C8E055DDD2CA}"/>
+    <workbookView xWindow="260" yWindow="1120" windowWidth="12620" windowHeight="11300"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="IO" sheetId="2" r:id="rId2"/>
     <sheet name="Alarms" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,127 +55,127 @@
     <t>four</t>
   </si>
   <si>
+    <t>posregs</t>
+  </si>
+  <si>
+    <t>pr1</t>
+  </si>
+  <si>
+    <t>pr2</t>
+  </si>
+  <si>
+    <t>pr3</t>
+  </si>
+  <si>
+    <t>pr4</t>
+  </si>
+  <si>
+    <t>pr5</t>
+  </si>
+  <si>
+    <t>ualm</t>
+  </si>
+  <si>
+    <t>test two</t>
+  </si>
+  <si>
+    <t>test three</t>
+  </si>
+  <si>
+    <t>test four</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>gi</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>ao</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>din1</t>
+  </si>
+  <si>
+    <t>din2</t>
+  </si>
+  <si>
+    <t>din3</t>
+  </si>
+  <si>
+    <t>dout1</t>
+  </si>
+  <si>
+    <t>dout2</t>
+  </si>
+  <si>
+    <t>dout3</t>
+  </si>
+  <si>
+    <t>dout4</t>
+  </si>
+  <si>
+    <t>rin1</t>
+  </si>
+  <si>
+    <t>rin2</t>
+  </si>
+  <si>
+    <t>rout1</t>
+  </si>
+  <si>
+    <t>gin1</t>
+  </si>
+  <si>
+    <t>gout1</t>
+  </si>
+  <si>
+    <t>ain1</t>
+  </si>
+  <si>
+    <t>aout1</t>
+  </si>
+  <si>
+    <t>sregs</t>
+  </si>
+  <si>
+    <t>sreg1</t>
+  </si>
+  <si>
+    <t>sreg2</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>this is an extremely long comment</t>
+  </si>
+  <si>
     <t>five</t>
-  </si>
-  <si>
-    <t>posregs</t>
-  </si>
-  <si>
-    <t>pr1</t>
-  </si>
-  <si>
-    <t>pr2</t>
-  </si>
-  <si>
-    <t>pr3</t>
-  </si>
-  <si>
-    <t>pr4</t>
-  </si>
-  <si>
-    <t>pr5</t>
-  </si>
-  <si>
-    <t>ualm</t>
-  </si>
-  <si>
-    <t>test two</t>
-  </si>
-  <si>
-    <t>test three</t>
-  </si>
-  <si>
-    <t>test four</t>
-  </si>
-  <si>
-    <t>ri</t>
-  </si>
-  <si>
-    <t>ro</t>
-  </si>
-  <si>
-    <t>gi</t>
-  </si>
-  <si>
-    <t>go</t>
-  </si>
-  <si>
-    <t>ai</t>
-  </si>
-  <si>
-    <t>ao</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>din1</t>
-  </si>
-  <si>
-    <t>din2</t>
-  </si>
-  <si>
-    <t>din3</t>
-  </si>
-  <si>
-    <t>dout1</t>
-  </si>
-  <si>
-    <t>dout2</t>
-  </si>
-  <si>
-    <t>dout3</t>
-  </si>
-  <si>
-    <t>dout4</t>
-  </si>
-  <si>
-    <t>rin1</t>
-  </si>
-  <si>
-    <t>rin2</t>
-  </si>
-  <si>
-    <t>rout1</t>
-  </si>
-  <si>
-    <t>gin1</t>
-  </si>
-  <si>
-    <t>gout1</t>
-  </si>
-  <si>
-    <t>ain1</t>
-  </si>
-  <si>
-    <t>aout1</t>
-  </si>
-  <si>
-    <t>sregs</t>
-  </si>
-  <si>
-    <t>sreg1</t>
-  </si>
-  <si>
-    <t>sreg2</t>
-  </si>
-  <si>
-    <t>flags</t>
-  </si>
-  <si>
-    <t>f1</t>
-  </si>
-  <si>
-    <t>this is an extremely long comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,16 +520,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2473686E-B083-42C4-A4C6-F56E03DA2EE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,51 +537,51 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -590,16 +592,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -610,10 +612,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -624,21 +626,21 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -647,131 +649,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173EB9B1-051D-4B2D-A86E-96559B44DA2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>34</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>37</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -780,21 +782,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA60EAB3-5286-4B68-99E6-FA4BB62064F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -802,28 +804,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>